<commit_message>
Commit medicine price calculation changes  - 25rd Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/data/medicine_inventory.xlsx
+++ b/src/steffs_pharmacy/data/medicine_inventory.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>

</xml_diff>